<commit_message>
set/get auction on group
</commit_message>
<xml_diff>
--- a/CricDream issue list.xlsx
+++ b/CricDream issue list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="19560" windowHeight="8340"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="19560" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>In login page, put our name in copyright "CricDream". Else put cricdream at top (in big font) and remove copy right</t>
+  </si>
+  <si>
+    <t>Not to be done. Ignore</t>
   </si>
 </sst>
 </file>
@@ -194,12 +197,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -214,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -239,6 +248,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -524,8 +536,8 @@
   <dimension ref="A2:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,14 +642,14 @@
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="5">
         <v>44081</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="6"/>
@@ -646,14 +658,14 @@
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="5">
         <v>44081</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="6"/>
@@ -669,10 +681,12 @@
         <v>44081</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="6"/>
+      <c r="F9" s="6" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -758,7 +772,7 @@
       <c r="A15" s="3">
         <v>13</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="5">
@@ -830,14 +844,14 @@
       <c r="A19" s="3">
         <v>17</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="5">
         <v>44081</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="6"/>

</xml_diff>

<commit_message>
C and VC added after player in myteam
</commit_message>
<xml_diff>
--- a/CricDream issue list.xlsx
+++ b/CricDream issue list.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="19560" windowHeight="8340"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="19560" windowHeight="8340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="9Sep2020" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$F$24</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="48">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -160,12 +161,66 @@
   <si>
     <t>Not to be done. Ignore</t>
   </si>
+  <si>
+    <t>Reconfirm message for sold</t>
+  </si>
+  <si>
+    <t>RHS to automatic hide after confirmed?</t>
+  </si>
+  <si>
+    <t>Cancel button in RHS along with Confirm</t>
+  </si>
+  <si>
+    <t>Stat to set to IPL2020</t>
+  </si>
+  <si>
+    <t>Admin to get Auction start button</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>Sold button to be disabled, if already purchased</t>
+  </si>
+  <si>
+    <t>Unsold to be implemented</t>
+  </si>
+  <si>
+    <t>Admin login test (apurva) on 9th September 2020</t>
+  </si>
+  <si>
+    <t>Check if (as user) My team shows purchased players</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>(admin) My team do not get all players sold</t>
+  </si>
+  <si>
+    <t>Extra Menu options to be added</t>
+  </si>
+  <si>
+    <t>Balance not getting updated for franchisee</t>
+  </si>
+  <si>
+    <t>Auction sequnce from PENDING to RUNNING working fine</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,6 +251,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -211,7 +274,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -219,11 +282,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -253,6 +331,33 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,9 +640,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,6 +1046,236 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+    </row>
+    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="5">
+        <v>44083</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>2</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="5">
+        <v>44081</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>3</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>4</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>5</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="20">
+        <v>6</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
+        <v>7</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
+        <v>8</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="20">
+        <v>9</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="18">
+        <v>10</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="18">
+        <v>11</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="16"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="18">
+        <v>12</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="16"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="18">
+        <v>13</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Sheet2!$A$1:$A$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3:E4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
scheduler chnaged. Rank new logic
</commit_message>
<xml_diff>
--- a/CricDream issue list.xlsx
+++ b/CricDream issue list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="19560" windowHeight="8340" activeTab="1"/>
+    <workbookView xWindow="4650" yWindow="0" windowWidth="19560" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="52">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -214,6 +214,18 @@
   </si>
   <si>
     <t>Auction sequnce from PENDING to RUNNING working fine</t>
+  </si>
+  <si>
+    <t>giving blank with value 0</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>Will show only unsold players</t>
+  </si>
+  <si>
+    <t>will skip to next player</t>
   </si>
 </sst>
 </file>
@@ -351,13 +363,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,9 +652,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,7 +698,7 @@
         <v>44081</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="6"/>
@@ -702,7 +714,7 @@
         <v>44081</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="6"/>
@@ -738,10 +750,12 @@
         <v>44081</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="6"/>
+      <c r="F6" s="6" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -757,7 +771,6 @@
         <v>4</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -804,7 +817,7 @@
         <v>44081</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="6"/>
@@ -868,7 +881,7 @@
         <v>44081</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="6"/>
@@ -884,7 +897,7 @@
         <v>44081</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E15" s="5">
         <v>44081</v>
@@ -904,7 +917,7 @@
         <v>44081</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="6"/>
@@ -936,7 +949,7 @@
         <v>44081</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E18" s="5">
         <v>44081</v>
@@ -1046,10 +1059,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,16 +1075,17 @@
     <col min="6" max="6" width="18.5703125" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="20.140625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-    </row>
-    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -1094,7 +1108,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -1112,8 +1126,14 @@
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>2</v>
       </c>
@@ -1132,7 +1152,7 @@
       <c r="F4" s="5"/>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <v>3</v>
       </c>
@@ -1143,7 +1163,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>4</v>
       </c>
@@ -1154,7 +1174,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>5</v>
       </c>
@@ -1164,22 +1184,25 @@
       <c r="C7" s="16" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="20">
+      <c r="I7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="19">
         <v>6</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="20" t="s">
         <v>36</v>
       </c>
       <c r="I8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>7</v>
       </c>
@@ -1189,8 +1212,14 @@
       <c r="C9" s="16" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>8</v>
       </c>
@@ -1200,22 +1229,25 @@
       <c r="C10" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="20">
+      <c r="I10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="19">
         <v>9</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="20" t="s">
         <v>38</v>
       </c>
       <c r="I11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="18">
         <v>10</v>
       </c>
@@ -1225,8 +1257,11 @@
       <c r="C12" s="17" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="18">
         <v>11</v>
       </c>
@@ -1235,7 +1270,7 @@
       </c>
       <c r="C13" s="16"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="18">
         <v>12</v>
       </c>
@@ -1243,8 +1278,11 @@
         <v>46</v>
       </c>
       <c r="C14" s="16"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="18">
         <v>13</v>
       </c>
@@ -1252,6 +1290,9 @@
         <v>47</v>
       </c>
       <c r="C15" s="16"/>
+      <c r="I15" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>